<commit_message>
Added many more sections to the LaTeX final report, with more corresponding images and changes made to various 'report_parts' files.
</commit_message>
<xml_diff>
--- a/report_stuff/Gantt chart.xlsx
+++ b/report_stuff/Gantt chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dheat\Dropbox\Imperial\Individual Project\indiv_proj\report_stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C39A64-3BFB-4FD2-AD59-0F210D4BEE08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B00045-0F67-41CD-9A8A-E946FCFB06F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{87C25B5A-2A69-4C36-A451-610E2188ED27}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{87C25B5A-2A69-4C36-A451-610E2188ED27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="274">
   <si>
     <t>Stage</t>
   </si>
@@ -781,6 +781,78 @@
   </si>
   <si>
     <t>Report: add to 'experiments and results discussions' a description of how experiment sets and MPS's are run</t>
+  </si>
+  <si>
+    <t>Report: write project timeline and Gantt chart</t>
+  </si>
+  <si>
+    <t>Add necessary 2 top-level READMEs as required by email</t>
+  </si>
+  <si>
+    <t>Report: write section on further improvements and project directions to undertake</t>
+  </si>
+  <si>
+    <t>Report (LaTeX): put together report parts 1.1 – 1.3 in LaTeX, including editing and spell check</t>
+  </si>
+  <si>
+    <t>Report (LaTeX): put together report parts 2.1 – 2.2 in LaTeX, including editing and spell check</t>
+  </si>
+  <si>
+    <t>MPS 23: Repeat single-act MPS but only using sensor magnetic field data and new model options</t>
+  </si>
+  <si>
+    <t>Report (LaTeX): put together report parts 3.1 – 3.2 in LaTeX, including editing and spell check</t>
+  </si>
+  <si>
+    <t>Write 'assess_nsaa_file.py' to run on final models (and extract necessary measurements) for given path and measurements</t>
+  </si>
+  <si>
+    <t>Remove and/or repurpose any excess batch scripts within 'batch_files'</t>
+  </si>
+  <si>
+    <t>Add 'assess_nsaa_file.py' README, update script explanations for this and for deleted batch scripts, and update diagram</t>
+  </si>
+  <si>
+    <t>Report (LaTeX): put together report parts 3.3 in LaTeX, including editing and spell check</t>
+  </si>
+  <si>
+    <t>Report (LaTeX): put together report parts 3.4 in LaTeX, including editing and spell check</t>
+  </si>
+  <si>
+    <t>Report (LaTeX): put together report parts 4.1 in LaTeX, including editing and spell check</t>
+  </si>
+  <si>
+    <t>Finish adding to 'Final Improvements'</t>
+  </si>
+  <si>
+    <t>Update OneDrive link for 'msc_project_files' with the final versions of all files</t>
+  </si>
+  <si>
+    <t>Report (LaTeX): put together report parts 5.2-5.3 in LaTeX, including editing and spell check</t>
+  </si>
+  <si>
+    <t>Report (LaTeX): add code to appendix</t>
+  </si>
+  <si>
+    <t>Report: add to 'Final evaluation results' section the final models used and the 'assess_' script</t>
+  </si>
+  <si>
+    <t>Report: add to 'Final evaluation results' conclusions from all experiments sets and MPS's (in particular 20-23)</t>
+  </si>
+  <si>
+    <t>Report (LaTeX): write 'Abstract', edit and include within LaTeX</t>
+  </si>
+  <si>
+    <t>Report (LaTex): add 'Literature Review' to report, including reviewing and editing</t>
+  </si>
+  <si>
+    <t>Report (LaTeX): add 'Conclusions' section of the report</t>
+  </si>
+  <si>
+    <t>MPS 22: Experiment w/ 'alt_dirs' with files trained on NSAA and predicting NMB files (AND vice versa)</t>
+  </si>
+  <si>
+    <t>Move final chosen models to directory within project directory, modify 'model_pred' to use these, and add to 'Final evaluation results'</t>
   </si>
 </sst>
 </file>
@@ -1226,10 +1298,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F13D08A-627D-4CC9-BA36-D72D5A6EDC3A}">
-  <dimension ref="D5:M251"/>
+  <dimension ref="D5:M275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E197" sqref="E197"/>
+    <sheetView tabSelected="1" topLeftCell="A211" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E236" sqref="E236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2570,7 +2642,7 @@
       <c r="E217" t="s">
         <v>240</v>
       </c>
-      <c r="H217" s="10"/>
+      <c r="I217" s="10"/>
     </row>
     <row r="218" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D218" t="s">
@@ -2579,7 +2651,7 @@
       <c r="E218" t="s">
         <v>151</v>
       </c>
-      <c r="H218" s="10"/>
+      <c r="I218" s="10"/>
     </row>
     <row r="219" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D219" t="s">
@@ -2588,7 +2660,7 @@
       <c r="E219" t="s">
         <v>152</v>
       </c>
-      <c r="H219" s="10"/>
+      <c r="I219" s="10"/>
     </row>
     <row r="220" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E220" t="s">
@@ -2648,55 +2720,55 @@
       <c r="E229" t="s">
         <v>209</v>
       </c>
-      <c r="I229" s="10"/>
+      <c r="J229" s="10"/>
     </row>
     <row r="230" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E230" t="s">
         <v>158</v>
       </c>
-      <c r="I230" s="10"/>
+      <c r="J230" s="10"/>
     </row>
     <row r="231" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E231" t="s">
         <v>210</v>
       </c>
-      <c r="I231" s="10"/>
+      <c r="J231" s="10"/>
     </row>
     <row r="232" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E232" t="s">
         <v>249</v>
       </c>
-      <c r="I232" s="10"/>
+      <c r="J232" s="10"/>
     </row>
     <row r="233" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E233" t="s">
         <v>159</v>
       </c>
-      <c r="I233" s="10"/>
+      <c r="J233" s="10"/>
     </row>
     <row r="234" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E234" t="s">
         <v>211</v>
       </c>
-      <c r="I234" s="10"/>
+      <c r="J234" s="10"/>
     </row>
     <row r="235" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E235" t="s">
         <v>160</v>
       </c>
-      <c r="I235" s="10"/>
+      <c r="J235" s="10"/>
     </row>
     <row r="236" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E236" t="s">
         <v>245</v>
       </c>
-      <c r="I236" s="10"/>
+      <c r="J236" s="10"/>
     </row>
     <row r="237" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E237" t="s">
         <v>241</v>
       </c>
-      <c r="I237" s="10"/>
+      <c r="J237" s="10"/>
     </row>
     <row r="238" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E238" t="s">
@@ -2716,71 +2788,215 @@
       </c>
       <c r="J240" s="10"/>
     </row>
-    <row r="241" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E241" t="s">
         <v>243</v>
       </c>
       <c r="J241" s="10"/>
     </row>
-    <row r="242" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E242" t="s">
         <v>244</v>
       </c>
       <c r="J242" s="10"/>
     </row>
-    <row r="243" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E243" t="s">
         <v>163</v>
       </c>
       <c r="J243" s="10"/>
     </row>
-    <row r="244" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E244" t="s">
         <v>164</v>
       </c>
       <c r="J244" s="10"/>
     </row>
-    <row r="245" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E245" t="s">
         <v>165</v>
       </c>
       <c r="J245" s="10"/>
     </row>
-    <row r="246" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E246" t="s">
         <v>166</v>
       </c>
       <c r="J246" s="10"/>
     </row>
-    <row r="247" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E247" t="s">
         <v>167</v>
       </c>
-      <c r="J247" s="10"/>
-    </row>
-    <row r="248" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K247" s="10"/>
+    </row>
+    <row r="248" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E248" t="s">
         <v>168</v>
       </c>
-      <c r="J248" s="10"/>
-    </row>
-    <row r="249" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K248" s="10"/>
+    </row>
+    <row r="249" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E249" t="s">
         <v>169</v>
       </c>
-      <c r="J249" s="10"/>
-    </row>
-    <row r="250" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K249" s="10"/>
+    </row>
+    <row r="250" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E250" t="s">
         <v>170</v>
       </c>
-      <c r="J250" s="10"/>
-    </row>
-    <row r="251" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K250" s="10"/>
+    </row>
+    <row r="251" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E251" t="s">
         <v>171</v>
       </c>
-      <c r="J251" s="10"/>
+      <c r="K251" s="10"/>
+    </row>
+    <row r="252" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E252" t="s">
+        <v>250</v>
+      </c>
+      <c r="K252" s="10"/>
+    </row>
+    <row r="253" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E253" t="s">
+        <v>251</v>
+      </c>
+      <c r="K253" s="10"/>
+    </row>
+    <row r="254" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E254" t="s">
+        <v>252</v>
+      </c>
+      <c r="K254" s="10"/>
+    </row>
+    <row r="255" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E255" t="s">
+        <v>253</v>
+      </c>
+      <c r="K255" s="10"/>
+    </row>
+    <row r="256" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E256" t="s">
+        <v>272</v>
+      </c>
+      <c r="K256" s="10"/>
+    </row>
+    <row r="257" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E257" t="s">
+        <v>254</v>
+      </c>
+      <c r="K257" s="10"/>
+    </row>
+    <row r="258" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E258" t="s">
+        <v>255</v>
+      </c>
+      <c r="K258" s="10"/>
+    </row>
+    <row r="259" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E259" t="s">
+        <v>256</v>
+      </c>
+      <c r="K259" s="10"/>
+    </row>
+    <row r="260" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E260" t="s">
+        <v>273</v>
+      </c>
+      <c r="K260" s="10"/>
+    </row>
+    <row r="261" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E261" t="s">
+        <v>257</v>
+      </c>
+      <c r="K261" s="10"/>
+    </row>
+    <row r="262" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E262" t="s">
+        <v>258</v>
+      </c>
+      <c r="K262" s="10"/>
+    </row>
+    <row r="263" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E263" t="s">
+        <v>259</v>
+      </c>
+      <c r="K263" s="10"/>
+    </row>
+    <row r="264" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E264" t="s">
+        <v>260</v>
+      </c>
+      <c r="K264" s="10"/>
+    </row>
+    <row r="265" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E265" t="s">
+        <v>261</v>
+      </c>
+      <c r="K265" s="10"/>
+    </row>
+    <row r="266" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E266" t="s">
+        <v>262</v>
+      </c>
+      <c r="L266" s="10"/>
+    </row>
+    <row r="267" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E267" t="s">
+        <v>263</v>
+      </c>
+      <c r="L267" s="10"/>
+    </row>
+    <row r="268" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E268" t="s">
+        <v>264</v>
+      </c>
+      <c r="L268" s="10"/>
+    </row>
+    <row r="269" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E269" t="s">
+        <v>265</v>
+      </c>
+      <c r="L269" s="10"/>
+    </row>
+    <row r="270" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E270" t="s">
+        <v>266</v>
+      </c>
+      <c r="L270" s="10"/>
+    </row>
+    <row r="271" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E271" t="s">
+        <v>267</v>
+      </c>
+      <c r="L271" s="10"/>
+    </row>
+    <row r="272" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E272" t="s">
+        <v>268</v>
+      </c>
+      <c r="L272" s="10"/>
+    </row>
+    <row r="273" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E273" t="s">
+        <v>269</v>
+      </c>
+      <c r="L273" s="10"/>
+    </row>
+    <row r="274" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E274" t="s">
+        <v>270</v>
+      </c>
+      <c r="L274" s="10"/>
+    </row>
+    <row r="275" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E275" t="s">
+        <v>271</v>
+      </c>
+      <c r="L275" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2789,21 +3005,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A78AC4AB812BE04F999A57EFC269C159" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="567be77a74f7705343e4192727575fae">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="05bb6ac5-9ba4-452c-9a0e-0b339f0a0afc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b6ec8f38eb45d86ebfbae85d4012c94" ns3:_="">
     <xsd:import namespace="05bb6ac5-9ba4-452c-9a0e-0b339f0a0afc"/>
@@ -2935,31 +3136,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D70C9ED9-CD8B-431E-97DF-3958A621B3F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="05bb6ac5-9ba4-452c-9a0e-0b339f0a0afc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35A31276-794F-4E51-B725-9E6965EC7C4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FB05DB3-5D69-4182-9427-A9ADFE57BD50}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2975,4 +3167,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35A31276-794F-4E51-B725-9E6965EC7C4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D70C9ED9-CD8B-431E-97DF-3958A621B3F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="05bb6ac5-9ba4-452c-9a0e-0b339f0a0afc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>